<commit_message>
intl tally modal done
</commit_message>
<xml_diff>
--- a/i18n.xlsx
+++ b/i18n.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/moneyPlanner/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83EE7AB0-EA0F-6E4A-9B57-A3A161EC0E9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28562564-C79E-D44B-9E0E-38B037012BF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="660" windowWidth="33600" windowHeight="17600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="900" yWindow="660" windowWidth="35700" windowHeight="17600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="i18n" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2052" uniqueCount="1098">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2152" uniqueCount="1152">
   <si>
     <t>locale_ref_id</t>
   </si>
@@ -3340,6 +3340,168 @@
   </si>
   <si>
     <t>رقم</t>
+  </si>
+  <si>
+    <t>solved</t>
+  </si>
+  <si>
+    <t>Solved</t>
+  </si>
+  <si>
+    <t>தீர்க்கப்பட்டது</t>
+  </si>
+  <si>
+    <t>Решено</t>
+  </si>
+  <si>
+    <t>Résolu</t>
+  </si>
+  <si>
+    <t>解决了</t>
+  </si>
+  <si>
+    <t>解決済み</t>
+  </si>
+  <si>
+    <t>Resolvido</t>
+  </si>
+  <si>
+    <t>हल किया</t>
+  </si>
+  <si>
+    <t>Resuelto</t>
+  </si>
+  <si>
+    <t>تم حلها</t>
+  </si>
+  <si>
+    <t>امام</t>
+  </si>
+  <si>
+    <t>ahead</t>
+  </si>
+  <si>
+    <t>Ahead</t>
+  </si>
+  <si>
+    <t>adelante</t>
+  </si>
+  <si>
+    <t>आगे</t>
+  </si>
+  <si>
+    <t>முன்னாடி</t>
+  </si>
+  <si>
+    <t>en avant</t>
+  </si>
+  <si>
+    <t>先</t>
+  </si>
+  <si>
+    <t>先に</t>
+  </si>
+  <si>
+    <t>à frente</t>
+  </si>
+  <si>
+    <t>предстоящий</t>
+  </si>
+  <si>
+    <t>tally</t>
+  </si>
+  <si>
+    <t>Tally</t>
+  </si>
+  <si>
+    <t>подсчитывать</t>
+  </si>
+  <si>
+    <t>contar</t>
+  </si>
+  <si>
+    <t>集計する</t>
+  </si>
+  <si>
+    <t>相符</t>
+  </si>
+  <si>
+    <t>எண்ணிக்கை</t>
+  </si>
+  <si>
+    <t>गणना</t>
+  </si>
+  <si>
+    <t>cuenta</t>
+  </si>
+  <si>
+    <t>حصيلة</t>
+  </si>
+  <si>
+    <t>unaccounted</t>
+  </si>
+  <si>
+    <t>Unaccounted</t>
+  </si>
+  <si>
+    <t>في عداد المفقودين</t>
+  </si>
+  <si>
+    <t>no contabilizado</t>
+  </si>
+  <si>
+    <t>बेहिसाब</t>
+  </si>
+  <si>
+    <t>கணக்கில் காட்டப்படாத</t>
+  </si>
+  <si>
+    <t>inexpliqué</t>
+  </si>
+  <si>
+    <t>下落不明</t>
+  </si>
+  <si>
+    <t>行方不明</t>
+  </si>
+  <si>
+    <t>não contabilizado</t>
+  </si>
+  <si>
+    <t>неучтенный</t>
+  </si>
+  <si>
+    <t>wallet</t>
+  </si>
+  <si>
+    <t>Wallet</t>
+  </si>
+  <si>
+    <t>Бумажник</t>
+  </si>
+  <si>
+    <t>Carteira</t>
+  </si>
+  <si>
+    <t>பணப்பை</t>
+  </si>
+  <si>
+    <t>Porte monnaie</t>
+  </si>
+  <si>
+    <t>钱包</t>
+  </si>
+  <si>
+    <t>財布</t>
+  </si>
+  <si>
+    <t>बटुआ</t>
+  </si>
+  <si>
+    <t>Cartera</t>
+  </si>
+  <si>
+    <t>محفظة</t>
   </si>
 </sst>
 </file>
@@ -4261,10 +4423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F1101"/>
+  <dimension ref="A1:F1151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1064" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D1096" sqref="D1096"/>
+    <sheetView tabSelected="1" topLeftCell="A1117" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D1144" sqref="D1144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -23797,7 +23959,7 @@
     </row>
     <row r="1028" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A1028">
-        <f t="shared" ref="A1028:A1091" si="33">A1027+1</f>
+        <f t="shared" ref="A1028:A1092" si="33">A1027+1</f>
         <v>1027</v>
       </c>
       <c r="B1028">
@@ -24817,7 +24979,7 @@
         <v>1082</v>
       </c>
       <c r="E1081" s="1" t="str">
-        <f t="shared" ref="E1081:E1091" si="34">CONCATENATE("(",CHAR(34),A1081,CHAR(34),",",CHAR(34),B1081,CHAR(34),",",CHAR(34),C1081,CHAR(34),",",CHAR(34),D1081,CHAR(34),"),")</f>
+        <f t="shared" ref="E1081:E1141" si="34">CONCATENATE("(",CHAR(34),A1081,CHAR(34),",",CHAR(34),B1081,CHAR(34),",",CHAR(34),C1081,CHAR(34),",",CHAR(34),D1081,CHAR(34),"),")</f>
         <v>("1080","10","yes","نعم"),</v>
       </c>
     </row>
@@ -25012,52 +25174,1002 @@
       </c>
     </row>
     <row r="1092" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E1092" s="1" t="s">
+      <c r="A1092">
+        <f t="shared" si="33"/>
+        <v>1091</v>
+      </c>
+      <c r="B1092">
+        <v>1</v>
+      </c>
+      <c r="C1092" s="4" t="s">
+        <v>1098</v>
+      </c>
+      <c r="D1092" s="4" t="s">
+        <v>1099</v>
+      </c>
+      <c r="E1092" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>("1091","1","solved","Solved"),</v>
+      </c>
+    </row>
+    <row r="1093" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1093">
+        <f t="shared" ref="A1093:A1141" si="35">A1092+1</f>
+        <v>1092</v>
+      </c>
+      <c r="B1093">
+        <v>2</v>
+      </c>
+      <c r="C1093" s="4" t="s">
+        <v>1098</v>
+      </c>
+      <c r="D1093" s="4" t="s">
+        <v>1100</v>
+      </c>
+      <c r="E1093" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>("1092","2","solved","தீர்க்கப்பட்டது"),</v>
+      </c>
+    </row>
+    <row r="1094" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1094">
+        <f t="shared" si="35"/>
+        <v>1093</v>
+      </c>
+      <c r="B1094">
+        <v>3</v>
+      </c>
+      <c r="C1094" s="4" t="s">
+        <v>1098</v>
+      </c>
+      <c r="D1094" s="4" t="s">
+        <v>1102</v>
+      </c>
+      <c r="E1094" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>("1093","3","solved","Résolu"),</v>
+      </c>
+    </row>
+    <row r="1095" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1095">
+        <f t="shared" si="35"/>
+        <v>1094</v>
+      </c>
+      <c r="B1095">
+        <v>4</v>
+      </c>
+      <c r="C1095" s="4" t="s">
+        <v>1098</v>
+      </c>
+      <c r="D1095" s="4" t="s">
+        <v>1103</v>
+      </c>
+      <c r="E1095" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>("1094","4","solved","解决了"),</v>
+      </c>
+    </row>
+    <row r="1096" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1096">
+        <f t="shared" si="35"/>
+        <v>1095</v>
+      </c>
+      <c r="B1096">
+        <v>5</v>
+      </c>
+      <c r="C1096" s="4" t="s">
+        <v>1098</v>
+      </c>
+      <c r="D1096" s="4" t="s">
+        <v>1104</v>
+      </c>
+      <c r="E1096" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>("1095","5","solved","解決済み"),</v>
+      </c>
+    </row>
+    <row r="1097" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1097">
+        <f t="shared" si="35"/>
+        <v>1096</v>
+      </c>
+      <c r="B1097">
+        <v>6</v>
+      </c>
+      <c r="C1097" s="4" t="s">
+        <v>1098</v>
+      </c>
+      <c r="D1097" s="4" t="s">
+        <v>1105</v>
+      </c>
+      <c r="E1097" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>("1096","6","solved","Resolvido"),</v>
+      </c>
+    </row>
+    <row r="1098" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1098">
+        <f t="shared" si="35"/>
+        <v>1097</v>
+      </c>
+      <c r="B1098">
+        <v>7</v>
+      </c>
+      <c r="C1098" s="4" t="s">
+        <v>1098</v>
+      </c>
+      <c r="D1098" s="4" t="s">
+        <v>1106</v>
+      </c>
+      <c r="E1098" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>("1097","7","solved","हल किया"),</v>
+      </c>
+    </row>
+    <row r="1099" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1099">
+        <f t="shared" si="35"/>
+        <v>1098</v>
+      </c>
+      <c r="B1099">
+        <v>8</v>
+      </c>
+      <c r="C1099" s="4" t="s">
+        <v>1098</v>
+      </c>
+      <c r="D1099" s="4" t="s">
+        <v>1101</v>
+      </c>
+      <c r="E1099" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>("1098","8","solved","Решено"),</v>
+      </c>
+    </row>
+    <row r="1100" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1100">
+        <f t="shared" si="35"/>
+        <v>1099</v>
+      </c>
+      <c r="B1100">
+        <v>9</v>
+      </c>
+      <c r="C1100" s="4" t="s">
+        <v>1098</v>
+      </c>
+      <c r="D1100" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="E1100" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>("1099","9","solved","Resuelto"),</v>
+      </c>
+    </row>
+    <row r="1101" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1101">
+        <f t="shared" si="35"/>
+        <v>1100</v>
+      </c>
+      <c r="B1101">
+        <v>10</v>
+      </c>
+      <c r="C1101" s="4" t="s">
+        <v>1098</v>
+      </c>
+      <c r="D1101" s="4" t="s">
+        <v>1108</v>
+      </c>
+      <c r="E1101" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>("1100","10","solved","تم حلها"),</v>
+      </c>
+    </row>
+    <row r="1102" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1102">
+        <f t="shared" si="35"/>
+        <v>1101</v>
+      </c>
+      <c r="B1102">
+        <v>1</v>
+      </c>
+      <c r="C1102" s="4" t="s">
+        <v>1110</v>
+      </c>
+      <c r="D1102" s="4" t="s">
+        <v>1111</v>
+      </c>
+      <c r="E1102" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>("1101","1","ahead","Ahead"),</v>
+      </c>
+    </row>
+    <row r="1103" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1103">
+        <f t="shared" si="35"/>
+        <v>1102</v>
+      </c>
+      <c r="B1103">
+        <v>2</v>
+      </c>
+      <c r="C1103" s="4" t="s">
+        <v>1110</v>
+      </c>
+      <c r="D1103" s="4" t="s">
+        <v>1114</v>
+      </c>
+      <c r="E1103" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>("1102","2","ahead","முன்னாடி"),</v>
+      </c>
+    </row>
+    <row r="1104" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1104">
+        <f t="shared" si="35"/>
+        <v>1103</v>
+      </c>
+      <c r="B1104">
+        <v>3</v>
+      </c>
+      <c r="C1104" s="4" t="s">
+        <v>1110</v>
+      </c>
+      <c r="D1104" s="4" t="s">
+        <v>1115</v>
+      </c>
+      <c r="E1104" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>("1103","3","ahead","en avant"),</v>
+      </c>
+    </row>
+    <row r="1105" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1105">
+        <f t="shared" si="35"/>
+        <v>1104</v>
+      </c>
+      <c r="B1105">
+        <v>4</v>
+      </c>
+      <c r="C1105" s="4" t="s">
+        <v>1110</v>
+      </c>
+      <c r="D1105" s="4" t="s">
+        <v>1116</v>
+      </c>
+      <c r="E1105" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>("1104","4","ahead","先"),</v>
+      </c>
+    </row>
+    <row r="1106" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1106">
+        <f t="shared" si="35"/>
+        <v>1105</v>
+      </c>
+      <c r="B1106">
+        <v>5</v>
+      </c>
+      <c r="C1106" s="4" t="s">
+        <v>1110</v>
+      </c>
+      <c r="D1106" s="4" t="s">
+        <v>1117</v>
+      </c>
+      <c r="E1106" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>("1105","5","ahead","先に"),</v>
+      </c>
+    </row>
+    <row r="1107" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1107">
+        <f t="shared" si="35"/>
+        <v>1106</v>
+      </c>
+      <c r="B1107">
+        <v>6</v>
+      </c>
+      <c r="C1107" s="4" t="s">
+        <v>1110</v>
+      </c>
+      <c r="D1107" s="4" t="s">
+        <v>1118</v>
+      </c>
+      <c r="E1107" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>("1106","6","ahead","à frente"),</v>
+      </c>
+    </row>
+    <row r="1108" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1108">
+        <f t="shared" si="35"/>
+        <v>1107</v>
+      </c>
+      <c r="B1108">
+        <v>7</v>
+      </c>
+      <c r="C1108" s="4" t="s">
+        <v>1110</v>
+      </c>
+      <c r="D1108" s="4" t="s">
+        <v>1113</v>
+      </c>
+      <c r="E1108" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>("1107","7","ahead","आगे"),</v>
+      </c>
+    </row>
+    <row r="1109" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1109">
+        <f t="shared" si="35"/>
+        <v>1108</v>
+      </c>
+      <c r="B1109">
+        <v>8</v>
+      </c>
+      <c r="C1109" s="4" t="s">
+        <v>1110</v>
+      </c>
+      <c r="D1109" s="4" t="s">
+        <v>1119</v>
+      </c>
+      <c r="E1109" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>("1108","8","ahead","предстоящий"),</v>
+      </c>
+    </row>
+    <row r="1110" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1110">
+        <f t="shared" si="35"/>
+        <v>1109</v>
+      </c>
+      <c r="B1110">
+        <v>9</v>
+      </c>
+      <c r="C1110" s="4" t="s">
+        <v>1110</v>
+      </c>
+      <c r="D1110" s="4" t="s">
+        <v>1112</v>
+      </c>
+      <c r="E1110" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>("1109","9","ahead","adelante"),</v>
+      </c>
+    </row>
+    <row r="1111" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1111">
+        <f t="shared" si="35"/>
+        <v>1110</v>
+      </c>
+      <c r="B1111">
+        <v>10</v>
+      </c>
+      <c r="C1111" s="4" t="s">
+        <v>1110</v>
+      </c>
+      <c r="D1111" s="4" t="s">
+        <v>1109</v>
+      </c>
+      <c r="E1111" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>("1110","10","ahead","امام"),</v>
+      </c>
+    </row>
+    <row r="1112" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1112">
+        <f t="shared" si="35"/>
+        <v>1111</v>
+      </c>
+      <c r="B1112">
+        <v>1</v>
+      </c>
+      <c r="C1112" s="4" t="s">
+        <v>1120</v>
+      </c>
+      <c r="D1112" s="4" t="s">
+        <v>1121</v>
+      </c>
+      <c r="E1112" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>("1111","1","tally","Tally"),</v>
+      </c>
+    </row>
+    <row r="1113" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1113">
+        <f t="shared" si="35"/>
+        <v>1112</v>
+      </c>
+      <c r="B1113">
+        <v>2</v>
+      </c>
+      <c r="C1113" s="4" t="s">
+        <v>1120</v>
+      </c>
+      <c r="D1113" s="4" t="s">
+        <v>1126</v>
+      </c>
+      <c r="E1113" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>("1112","2","tally","எண்ணிக்கை"),</v>
+      </c>
+    </row>
+    <row r="1114" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1114">
+        <f t="shared" si="35"/>
+        <v>1113</v>
+      </c>
+      <c r="B1114">
+        <v>3</v>
+      </c>
+      <c r="C1114" s="4" t="s">
+        <v>1120</v>
+      </c>
+      <c r="D1114" s="4" t="s">
+        <v>1126</v>
+      </c>
+      <c r="E1114" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>("1113","3","tally","எண்ணிக்கை"),</v>
+      </c>
+    </row>
+    <row r="1115" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1115">
+        <f t="shared" si="35"/>
+        <v>1114</v>
+      </c>
+      <c r="B1115">
+        <v>4</v>
+      </c>
+      <c r="C1115" s="4" t="s">
+        <v>1120</v>
+      </c>
+      <c r="D1115" s="4" t="s">
+        <v>1125</v>
+      </c>
+      <c r="E1115" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>("1114","4","tally","相符"),</v>
+      </c>
+    </row>
+    <row r="1116" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1116">
+        <f t="shared" si="35"/>
+        <v>1115</v>
+      </c>
+      <c r="B1116">
+        <v>5</v>
+      </c>
+      <c r="C1116" s="4" t="s">
+        <v>1120</v>
+      </c>
+      <c r="D1116" s="4" t="s">
+        <v>1124</v>
+      </c>
+      <c r="E1116" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>("1115","5","tally","集計する"),</v>
+      </c>
+    </row>
+    <row r="1117" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1117">
+        <f t="shared" si="35"/>
+        <v>1116</v>
+      </c>
+      <c r="B1117">
+        <v>6</v>
+      </c>
+      <c r="C1117" s="4" t="s">
+        <v>1120</v>
+      </c>
+      <c r="D1117" s="4" t="s">
+        <v>1123</v>
+      </c>
+      <c r="E1117" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>("1116","6","tally","contar"),</v>
+      </c>
+    </row>
+    <row r="1118" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1118">
+        <f t="shared" si="35"/>
+        <v>1117</v>
+      </c>
+      <c r="B1118">
+        <v>7</v>
+      </c>
+      <c r="C1118" s="4" t="s">
+        <v>1120</v>
+      </c>
+      <c r="D1118" s="4" t="s">
+        <v>1127</v>
+      </c>
+      <c r="E1118" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>("1117","7","tally","गणना"),</v>
+      </c>
+    </row>
+    <row r="1119" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1119">
+        <f t="shared" si="35"/>
+        <v>1118</v>
+      </c>
+      <c r="B1119">
+        <v>8</v>
+      </c>
+      <c r="C1119" s="4" t="s">
+        <v>1120</v>
+      </c>
+      <c r="D1119" s="4" t="s">
+        <v>1122</v>
+      </c>
+      <c r="E1119" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>("1118","8","tally","подсчитывать"),</v>
+      </c>
+    </row>
+    <row r="1120" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1120">
+        <f t="shared" si="35"/>
+        <v>1119</v>
+      </c>
+      <c r="B1120">
+        <v>9</v>
+      </c>
+      <c r="C1120" s="4" t="s">
+        <v>1120</v>
+      </c>
+      <c r="D1120" s="4" t="s">
+        <v>1128</v>
+      </c>
+      <c r="E1120" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>("1119","9","tally","cuenta"),</v>
+      </c>
+    </row>
+    <row r="1121" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1121">
+        <f t="shared" si="35"/>
+        <v>1120</v>
+      </c>
+      <c r="B1121">
+        <v>10</v>
+      </c>
+      <c r="C1121" s="4" t="s">
+        <v>1120</v>
+      </c>
+      <c r="D1121" s="4" t="s">
+        <v>1129</v>
+      </c>
+      <c r="E1121" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>("1120","10","tally","حصيلة"),</v>
+      </c>
+    </row>
+    <row r="1122" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1122">
+        <f t="shared" si="35"/>
+        <v>1121</v>
+      </c>
+      <c r="B1122">
+        <v>1</v>
+      </c>
+      <c r="C1122" s="4" t="s">
+        <v>1130</v>
+      </c>
+      <c r="D1122" s="4" t="s">
+        <v>1131</v>
+      </c>
+      <c r="E1122" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>("1121","1","unaccounted","Unaccounted"),</v>
+      </c>
+    </row>
+    <row r="1123" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1123">
+        <f t="shared" si="35"/>
+        <v>1122</v>
+      </c>
+      <c r="B1123">
+        <v>2</v>
+      </c>
+      <c r="C1123" s="4" t="s">
+        <v>1130</v>
+      </c>
+      <c r="D1123" s="4" t="s">
+        <v>1135</v>
+      </c>
+      <c r="E1123" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>("1122","2","unaccounted","கணக்கில் காட்டப்படாத"),</v>
+      </c>
+    </row>
+    <row r="1124" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1124">
+        <f t="shared" si="35"/>
+        <v>1123</v>
+      </c>
+      <c r="B1124">
+        <v>3</v>
+      </c>
+      <c r="C1124" s="4" t="s">
+        <v>1130</v>
+      </c>
+      <c r="D1124" s="4" t="s">
+        <v>1136</v>
+      </c>
+      <c r="E1124" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>("1123","3","unaccounted","inexpliqué"),</v>
+      </c>
+    </row>
+    <row r="1125" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1125">
+        <f t="shared" si="35"/>
+        <v>1124</v>
+      </c>
+      <c r="B1125">
+        <v>4</v>
+      </c>
+      <c r="C1125" s="4" t="s">
+        <v>1130</v>
+      </c>
+      <c r="D1125" s="4" t="s">
+        <v>1137</v>
+      </c>
+      <c r="E1125" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>("1124","4","unaccounted","下落不明"),</v>
+      </c>
+    </row>
+    <row r="1126" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1126">
+        <f t="shared" si="35"/>
+        <v>1125</v>
+      </c>
+      <c r="B1126">
+        <v>5</v>
+      </c>
+      <c r="C1126" s="4" t="s">
+        <v>1130</v>
+      </c>
+      <c r="D1126" s="4" t="s">
+        <v>1138</v>
+      </c>
+      <c r="E1126" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>("1125","5","unaccounted","行方不明"),</v>
+      </c>
+    </row>
+    <row r="1127" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1127">
+        <f t="shared" si="35"/>
+        <v>1126</v>
+      </c>
+      <c r="B1127">
+        <v>6</v>
+      </c>
+      <c r="C1127" s="4" t="s">
+        <v>1130</v>
+      </c>
+      <c r="D1127" s="4" t="s">
+        <v>1139</v>
+      </c>
+      <c r="E1127" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>("1126","6","unaccounted","não contabilizado"),</v>
+      </c>
+    </row>
+    <row r="1128" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1128">
+        <f t="shared" si="35"/>
+        <v>1127</v>
+      </c>
+      <c r="B1128">
+        <v>7</v>
+      </c>
+      <c r="C1128" s="4" t="s">
+        <v>1130</v>
+      </c>
+      <c r="D1128" s="4" t="s">
+        <v>1134</v>
+      </c>
+      <c r="E1128" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>("1127","7","unaccounted","बेहिसाब"),</v>
+      </c>
+    </row>
+    <row r="1129" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1129">
+        <f t="shared" si="35"/>
+        <v>1128</v>
+      </c>
+      <c r="B1129">
+        <v>8</v>
+      </c>
+      <c r="C1129" s="4" t="s">
+        <v>1130</v>
+      </c>
+      <c r="D1129" s="4" t="s">
+        <v>1140</v>
+      </c>
+      <c r="E1129" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>("1128","8","unaccounted","неучтенный"),</v>
+      </c>
+    </row>
+    <row r="1130" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1130">
+        <f t="shared" si="35"/>
+        <v>1129</v>
+      </c>
+      <c r="B1130">
+        <v>9</v>
+      </c>
+      <c r="C1130" s="4" t="s">
+        <v>1130</v>
+      </c>
+      <c r="D1130" s="4" t="s">
+        <v>1133</v>
+      </c>
+      <c r="E1130" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>("1129","9","unaccounted","no contabilizado"),</v>
+      </c>
+    </row>
+    <row r="1131" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1131">
+        <f t="shared" si="35"/>
+        <v>1130</v>
+      </c>
+      <c r="B1131">
+        <v>10</v>
+      </c>
+      <c r="C1131" s="4" t="s">
+        <v>1130</v>
+      </c>
+      <c r="D1131" s="4" t="s">
+        <v>1132</v>
+      </c>
+      <c r="E1131" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>("1130","10","unaccounted","في عداد المفقودين"),</v>
+      </c>
+    </row>
+    <row r="1132" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1132">
+        <f t="shared" si="35"/>
+        <v>1131</v>
+      </c>
+      <c r="B1132">
+        <v>1</v>
+      </c>
+      <c r="C1132" s="4" t="s">
+        <v>1141</v>
+      </c>
+      <c r="D1132" s="4" t="s">
+        <v>1142</v>
+      </c>
+      <c r="E1132" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>("1131","1","wallet","Wallet"),</v>
+      </c>
+    </row>
+    <row r="1133" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1133">
+        <f t="shared" si="35"/>
+        <v>1132</v>
+      </c>
+      <c r="B1133">
+        <v>2</v>
+      </c>
+      <c r="C1133" s="4" t="s">
+        <v>1141</v>
+      </c>
+      <c r="D1133" s="4" t="s">
+        <v>1145</v>
+      </c>
+      <c r="E1133" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>("1132","2","wallet","பணப்பை"),</v>
+      </c>
+    </row>
+    <row r="1134" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1134">
+        <f t="shared" si="35"/>
+        <v>1133</v>
+      </c>
+      <c r="B1134">
+        <v>3</v>
+      </c>
+      <c r="C1134" s="4" t="s">
+        <v>1141</v>
+      </c>
+      <c r="D1134" s="4" t="s">
+        <v>1146</v>
+      </c>
+      <c r="E1134" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>("1133","3","wallet","Porte monnaie"),</v>
+      </c>
+    </row>
+    <row r="1135" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1135">
+        <f t="shared" si="35"/>
+        <v>1134</v>
+      </c>
+      <c r="B1135">
+        <v>4</v>
+      </c>
+      <c r="C1135" s="4" t="s">
+        <v>1141</v>
+      </c>
+      <c r="D1135" s="4" t="s">
+        <v>1147</v>
+      </c>
+      <c r="E1135" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>("1134","4","wallet","钱包"),</v>
+      </c>
+    </row>
+    <row r="1136" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1136">
+        <f t="shared" si="35"/>
+        <v>1135</v>
+      </c>
+      <c r="B1136">
+        <v>5</v>
+      </c>
+      <c r="C1136" s="4" t="s">
+        <v>1141</v>
+      </c>
+      <c r="D1136" s="4" t="s">
+        <v>1148</v>
+      </c>
+      <c r="E1136" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>("1135","5","wallet","財布"),</v>
+      </c>
+    </row>
+    <row r="1137" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1137">
+        <f t="shared" si="35"/>
+        <v>1136</v>
+      </c>
+      <c r="B1137">
+        <v>6</v>
+      </c>
+      <c r="C1137" s="4" t="s">
+        <v>1141</v>
+      </c>
+      <c r="D1137" s="4" t="s">
+        <v>1144</v>
+      </c>
+      <c r="E1137" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>("1136","6","wallet","Carteira"),</v>
+      </c>
+    </row>
+    <row r="1138" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1138">
+        <f t="shared" si="35"/>
+        <v>1137</v>
+      </c>
+      <c r="B1138">
+        <v>7</v>
+      </c>
+      <c r="C1138" s="4" t="s">
+        <v>1141</v>
+      </c>
+      <c r="D1138" s="4" t="s">
+        <v>1149</v>
+      </c>
+      <c r="E1138" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>("1137","7","wallet","बटुआ"),</v>
+      </c>
+    </row>
+    <row r="1139" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1139">
+        <f t="shared" si="35"/>
+        <v>1138</v>
+      </c>
+      <c r="B1139">
+        <v>8</v>
+      </c>
+      <c r="C1139" s="4" t="s">
+        <v>1141</v>
+      </c>
+      <c r="D1139" s="4" t="s">
+        <v>1143</v>
+      </c>
+      <c r="E1139" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>("1138","8","wallet","Бумажник"),</v>
+      </c>
+    </row>
+    <row r="1140" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1140">
+        <f t="shared" si="35"/>
+        <v>1139</v>
+      </c>
+      <c r="B1140">
+        <v>9</v>
+      </c>
+      <c r="C1140" s="4" t="s">
+        <v>1141</v>
+      </c>
+      <c r="D1140" s="4" t="s">
+        <v>1150</v>
+      </c>
+      <c r="E1140" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>("1139","9","wallet","Cartera"),</v>
+      </c>
+    </row>
+    <row r="1141" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1141">
+        <f t="shared" si="35"/>
+        <v>1140</v>
+      </c>
+      <c r="B1141">
+        <v>10</v>
+      </c>
+      <c r="C1141" s="4" t="s">
+        <v>1141</v>
+      </c>
+      <c r="D1141" s="4" t="s">
+        <v>1151</v>
+      </c>
+      <c r="E1141" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>("1140","10","wallet","محفظة"),</v>
+      </c>
+    </row>
+    <row r="1142" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E1142" s="1" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="1093" spans="1:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="E1093" s="5" t="s">
+    <row r="1143" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="E1143" s="5" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="1094" spans="1:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="E1094" s="5" t="s">
+    <row r="1144" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="E1144" s="5" t="s">
         <v>519</v>
       </c>
     </row>
-    <row r="1095" spans="1:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="E1095" s="5" t="s">
+    <row r="1145" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="E1145" s="5" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="1096" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E1096" s="4" t="s">
+    <row r="1146" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E1146" s="4" t="s">
         <v>1042</v>
       </c>
     </row>
-    <row r="1097" spans="1:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="E1097" s="5" t="s">
+    <row r="1147" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="E1147" s="5" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="1098" spans="1:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="E1098" s="5" t="s">
+    <row r="1148" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="E1148" s="5" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="1099" spans="1:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="E1099" s="5" t="s">
+    <row r="1149" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="E1149" s="5" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="1100" spans="1:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="E1100" s="5" t="s">
+    <row r="1150" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="E1150" s="5" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="1101" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E1101" s="1" t="s">
+    <row r="1151" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E1151" s="1" t="s">
         <v>675</v>
       </c>
     </row>

</xml_diff>

<commit_message>
income chart legend added
</commit_message>
<xml_diff>
--- a/i18n.xlsx
+++ b/i18n.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/moneyPlanner/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CC6D329-8EB0-D343-8076-1992A06CE5F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{519E1FFF-5CB9-B643-AAC1-A320866AFFE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1780" yWindow="500" windowWidth="33600" windowHeight="19040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="i18n" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7452" uniqueCount="3962">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7552" uniqueCount="4014">
   <si>
     <t>locale_ref_id</t>
   </si>
@@ -11943,6 +11943,162 @@
   </si>
   <si>
     <t>طاولة الرقيق</t>
+  </si>
+  <si>
+    <t>highest</t>
+  </si>
+  <si>
+    <t>lowest</t>
+  </si>
+  <si>
+    <t>daily</t>
+  </si>
+  <si>
+    <t>hourly</t>
+  </si>
+  <si>
+    <t>weekly</t>
+  </si>
+  <si>
+    <t>Highest</t>
+  </si>
+  <si>
+    <t>மிக உயர்ந்தது</t>
+  </si>
+  <si>
+    <t>最高</t>
+  </si>
+  <si>
+    <t>الأعلى</t>
+  </si>
+  <si>
+    <t>le plus élevé</t>
+  </si>
+  <si>
+    <t>Altíssima</t>
+  </si>
+  <si>
+    <t>उच्चतम</t>
+  </si>
+  <si>
+    <t>наибольший</t>
+  </si>
+  <si>
+    <t>Mas alto</t>
+  </si>
+  <si>
+    <t>Lowest</t>
+  </si>
+  <si>
+    <t>El mas bajo</t>
+  </si>
+  <si>
+    <t>самый низкий</t>
+  </si>
+  <si>
+    <t>सबसे कम</t>
+  </si>
+  <si>
+    <t>குறைந்த</t>
+  </si>
+  <si>
+    <t>le plus bas</t>
+  </si>
+  <si>
+    <t>最低</t>
+  </si>
+  <si>
+    <t>mais baixo</t>
+  </si>
+  <si>
+    <t>أدنى</t>
+  </si>
+  <si>
+    <t>Daily</t>
+  </si>
+  <si>
+    <t>اليومي</t>
+  </si>
+  <si>
+    <t>diário</t>
+  </si>
+  <si>
+    <t>毎日</t>
+  </si>
+  <si>
+    <t>தினசரி</t>
+  </si>
+  <si>
+    <t>du quotidien</t>
+  </si>
+  <si>
+    <t>日常的</t>
+  </si>
+  <si>
+    <t>रोज</t>
+  </si>
+  <si>
+    <t>повседневная</t>
+  </si>
+  <si>
+    <t>Diario</t>
+  </si>
+  <si>
+    <t>Hourly</t>
+  </si>
+  <si>
+    <t>cada hora</t>
+  </si>
+  <si>
+    <t>ежечасно</t>
+  </si>
+  <si>
+    <t>प्रति घंटा</t>
+  </si>
+  <si>
+    <t xml:space="preserve">மணிக்கு </t>
+  </si>
+  <si>
+    <t>toutes les heures</t>
+  </si>
+  <si>
+    <t>每小时</t>
+  </si>
+  <si>
+    <t>毎時</t>
+  </si>
+  <si>
+    <t>de hora em hora</t>
+  </si>
+  <si>
+    <t>ساعيا</t>
+  </si>
+  <si>
+    <t>Weekly</t>
+  </si>
+  <si>
+    <t>أسبوعي</t>
+  </si>
+  <si>
+    <t>semanalmente</t>
+  </si>
+  <si>
+    <t>毎週</t>
+  </si>
+  <si>
+    <t>வாரந்தோறும்</t>
+  </si>
+  <si>
+    <t>hebdomadaire</t>
+  </si>
+  <si>
+    <t>每周</t>
+  </si>
+  <si>
+    <t>साप्ताहिक</t>
+  </si>
+  <si>
+    <t>еженедельно</t>
   </si>
 </sst>
 </file>
@@ -12894,10 +13050,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F3801"/>
+  <dimension ref="A1:F3851"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3775" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D3797" sqref="D3797"/>
+    <sheetView tabSelected="1" topLeftCell="A3818" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E3846" sqref="E3846"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -84512,7 +84668,7 @@
     </row>
     <row r="3769" spans="1:5">
       <c r="A3769">
-        <f t="shared" ref="A3769:A3791" si="119">A3768+1</f>
+        <f t="shared" ref="A3769:A3832" si="119">A3768+1</f>
         <v>3768</v>
       </c>
       <c r="B3769" s="13">
@@ -84525,7 +84681,7 @@
         <v>3915</v>
       </c>
       <c r="E3769" t="str">
-        <f t="shared" ref="E3769:E3791" si="120">CONCATENATE("(",CHAR(34),A3769,CHAR(34),",",CHAR(34),B3769,CHAR(34),",",CHAR(34),C3769,CHAR(34),",",CHAR(34),D3769,CHAR(34),"),")</f>
+        <f t="shared" ref="E3769:E3832" si="120">CONCATENATE("(",CHAR(34),A3769,CHAR(34),",",CHAR(34),B3769,CHAR(34),",",CHAR(34),C3769,CHAR(34),",",CHAR(34),D3769,CHAR(34),"),")</f>
         <v>("3768","8","indentOfIntlForm","Отступ этой формы предназначен для редактирования значений языка и добавления новых языков по вашему желанию."),</v>
       </c>
     </row>
@@ -84948,52 +85104,1002 @@
       </c>
     </row>
     <row r="3792" spans="1:5">
-      <c r="E3792" t="s">
+      <c r="A3792">
+        <f t="shared" si="119"/>
+        <v>3791</v>
+      </c>
+      <c r="B3792" s="13">
+        <v>1</v>
+      </c>
+      <c r="C3792" t="s">
+        <v>3962</v>
+      </c>
+      <c r="D3792" s="6" t="s">
+        <v>3967</v>
+      </c>
+      <c r="E3792" t="str">
+        <f t="shared" si="120"/>
+        <v>("3791","1","highest","Highest"),</v>
+      </c>
+    </row>
+    <row r="3793" spans="1:5">
+      <c r="A3793">
+        <f t="shared" si="119"/>
+        <v>3792</v>
+      </c>
+      <c r="B3793" s="13">
+        <v>2</v>
+      </c>
+      <c r="C3793" t="s">
+        <v>3962</v>
+      </c>
+      <c r="D3793" s="6" t="s">
+        <v>3968</v>
+      </c>
+      <c r="E3793" t="str">
+        <f t="shared" si="120"/>
+        <v>("3792","2","highest","மிக உயர்ந்தது"),</v>
+      </c>
+    </row>
+    <row r="3794" spans="1:5">
+      <c r="A3794">
+        <f t="shared" si="119"/>
+        <v>3793</v>
+      </c>
+      <c r="B3794" s="13">
+        <v>3</v>
+      </c>
+      <c r="C3794" t="s">
+        <v>3962</v>
+      </c>
+      <c r="D3794" s="6" t="s">
+        <v>3971</v>
+      </c>
+      <c r="E3794" t="str">
+        <f t="shared" si="120"/>
+        <v>("3793","3","highest","le plus élevé"),</v>
+      </c>
+    </row>
+    <row r="3795" spans="1:5">
+      <c r="A3795">
+        <f t="shared" si="119"/>
+        <v>3794</v>
+      </c>
+      <c r="B3795" s="13">
+        <v>4</v>
+      </c>
+      <c r="C3795" t="s">
+        <v>3962</v>
+      </c>
+      <c r="D3795" s="6" t="s">
+        <v>3969</v>
+      </c>
+      <c r="E3795" t="str">
+        <f t="shared" si="120"/>
+        <v>("3794","4","highest","最高"),</v>
+      </c>
+    </row>
+    <row r="3796" spans="1:5">
+      <c r="A3796">
+        <f t="shared" si="119"/>
+        <v>3795</v>
+      </c>
+      <c r="B3796" s="13">
+        <v>5</v>
+      </c>
+      <c r="C3796" t="s">
+        <v>3962</v>
+      </c>
+      <c r="D3796" s="6" t="s">
+        <v>3969</v>
+      </c>
+      <c r="E3796" t="str">
+        <f t="shared" si="120"/>
+        <v>("3795","5","highest","最高"),</v>
+      </c>
+    </row>
+    <row r="3797" spans="1:5">
+      <c r="A3797">
+        <f t="shared" si="119"/>
+        <v>3796</v>
+      </c>
+      <c r="B3797" s="13">
+        <v>6</v>
+      </c>
+      <c r="C3797" t="s">
+        <v>3962</v>
+      </c>
+      <c r="D3797" s="6" t="s">
+        <v>3972</v>
+      </c>
+      <c r="E3797" t="str">
+        <f t="shared" si="120"/>
+        <v>("3796","6","highest","Altíssima"),</v>
+      </c>
+    </row>
+    <row r="3798" spans="1:5">
+      <c r="A3798">
+        <f t="shared" si="119"/>
+        <v>3797</v>
+      </c>
+      <c r="B3798" s="13">
+        <v>7</v>
+      </c>
+      <c r="C3798" t="s">
+        <v>3962</v>
+      </c>
+      <c r="D3798" s="6" t="s">
+        <v>3973</v>
+      </c>
+      <c r="E3798" t="str">
+        <f t="shared" si="120"/>
+        <v>("3797","7","highest","उच्चतम"),</v>
+      </c>
+    </row>
+    <row r="3799" spans="1:5">
+      <c r="A3799">
+        <f t="shared" si="119"/>
+        <v>3798</v>
+      </c>
+      <c r="B3799" s="13">
+        <v>8</v>
+      </c>
+      <c r="C3799" t="s">
+        <v>3962</v>
+      </c>
+      <c r="D3799" s="6" t="s">
+        <v>3974</v>
+      </c>
+      <c r="E3799" t="str">
+        <f t="shared" si="120"/>
+        <v>("3798","8","highest","наибольший"),</v>
+      </c>
+    </row>
+    <row r="3800" spans="1:5">
+      <c r="A3800">
+        <f t="shared" si="119"/>
+        <v>3799</v>
+      </c>
+      <c r="B3800" s="13">
+        <v>9</v>
+      </c>
+      <c r="C3800" t="s">
+        <v>3962</v>
+      </c>
+      <c r="D3800" s="6" t="s">
+        <v>3975</v>
+      </c>
+      <c r="E3800" t="str">
+        <f t="shared" si="120"/>
+        <v>("3799","9","highest","Mas alto"),</v>
+      </c>
+    </row>
+    <row r="3801" spans="1:5">
+      <c r="A3801">
+        <f t="shared" si="119"/>
+        <v>3800</v>
+      </c>
+      <c r="B3801" s="13">
+        <v>10</v>
+      </c>
+      <c r="C3801" t="s">
+        <v>3962</v>
+      </c>
+      <c r="D3801" s="6" t="s">
+        <v>3970</v>
+      </c>
+      <c r="E3801" t="str">
+        <f t="shared" si="120"/>
+        <v>("3800","10","highest","الأعلى"),</v>
+      </c>
+    </row>
+    <row r="3802" spans="1:5">
+      <c r="A3802">
+        <f t="shared" si="119"/>
+        <v>3801</v>
+      </c>
+      <c r="B3802" s="13">
+        <v>1</v>
+      </c>
+      <c r="C3802" t="s">
+        <v>3963</v>
+      </c>
+      <c r="D3802" s="6" t="s">
+        <v>3976</v>
+      </c>
+      <c r="E3802" t="str">
+        <f t="shared" si="120"/>
+        <v>("3801","1","lowest","Lowest"),</v>
+      </c>
+    </row>
+    <row r="3803" spans="1:5">
+      <c r="A3803">
+        <f t="shared" si="119"/>
+        <v>3802</v>
+      </c>
+      <c r="B3803" s="13">
+        <v>2</v>
+      </c>
+      <c r="C3803" t="s">
+        <v>3963</v>
+      </c>
+      <c r="D3803" s="6" t="s">
+        <v>3980</v>
+      </c>
+      <c r="E3803" t="str">
+        <f t="shared" si="120"/>
+        <v>("3802","2","lowest","குறைந்த"),</v>
+      </c>
+    </row>
+    <row r="3804" spans="1:5">
+      <c r="A3804">
+        <f t="shared" si="119"/>
+        <v>3803</v>
+      </c>
+      <c r="B3804" s="13">
+        <v>3</v>
+      </c>
+      <c r="C3804" t="s">
+        <v>3963</v>
+      </c>
+      <c r="D3804" s="6" t="s">
+        <v>3981</v>
+      </c>
+      <c r="E3804" t="str">
+        <f t="shared" si="120"/>
+        <v>("3803","3","lowest","le plus bas"),</v>
+      </c>
+    </row>
+    <row r="3805" spans="1:5">
+      <c r="A3805">
+        <f t="shared" si="119"/>
+        <v>3804</v>
+      </c>
+      <c r="B3805" s="13">
+        <v>4</v>
+      </c>
+      <c r="C3805" t="s">
+        <v>3963</v>
+      </c>
+      <c r="D3805" s="6" t="s">
+        <v>3982</v>
+      </c>
+      <c r="E3805" t="str">
+        <f t="shared" si="120"/>
+        <v>("3804","4","lowest","最低"),</v>
+      </c>
+    </row>
+    <row r="3806" spans="1:5">
+      <c r="A3806">
+        <f t="shared" si="119"/>
+        <v>3805</v>
+      </c>
+      <c r="B3806" s="13">
+        <v>5</v>
+      </c>
+      <c r="C3806" t="s">
+        <v>3963</v>
+      </c>
+      <c r="D3806" s="6" t="s">
+        <v>3982</v>
+      </c>
+      <c r="E3806" t="str">
+        <f t="shared" si="120"/>
+        <v>("3805","5","lowest","最低"),</v>
+      </c>
+    </row>
+    <row r="3807" spans="1:5">
+      <c r="A3807">
+        <f t="shared" si="119"/>
+        <v>3806</v>
+      </c>
+      <c r="B3807" s="13">
+        <v>6</v>
+      </c>
+      <c r="C3807" t="s">
+        <v>3963</v>
+      </c>
+      <c r="D3807" s="6" t="s">
+        <v>3983</v>
+      </c>
+      <c r="E3807" t="str">
+        <f t="shared" si="120"/>
+        <v>("3806","6","lowest","mais baixo"),</v>
+      </c>
+    </row>
+    <row r="3808" spans="1:5">
+      <c r="A3808">
+        <f t="shared" si="119"/>
+        <v>3807</v>
+      </c>
+      <c r="B3808" s="13">
+        <v>7</v>
+      </c>
+      <c r="C3808" t="s">
+        <v>3963</v>
+      </c>
+      <c r="D3808" s="6" t="s">
+        <v>3979</v>
+      </c>
+      <c r="E3808" t="str">
+        <f t="shared" si="120"/>
+        <v>("3807","7","lowest","सबसे कम"),</v>
+      </c>
+    </row>
+    <row r="3809" spans="1:5">
+      <c r="A3809">
+        <f t="shared" si="119"/>
+        <v>3808</v>
+      </c>
+      <c r="B3809" s="13">
+        <v>8</v>
+      </c>
+      <c r="C3809" t="s">
+        <v>3963</v>
+      </c>
+      <c r="D3809" s="6" t="s">
+        <v>3978</v>
+      </c>
+      <c r="E3809" t="str">
+        <f t="shared" si="120"/>
+        <v>("3808","8","lowest","самый низкий"),</v>
+      </c>
+    </row>
+    <row r="3810" spans="1:5">
+      <c r="A3810">
+        <f t="shared" si="119"/>
+        <v>3809</v>
+      </c>
+      <c r="B3810" s="13">
+        <v>9</v>
+      </c>
+      <c r="C3810" t="s">
+        <v>3963</v>
+      </c>
+      <c r="D3810" s="6" t="s">
+        <v>3977</v>
+      </c>
+      <c r="E3810" t="str">
+        <f t="shared" si="120"/>
+        <v>("3809","9","lowest","El mas bajo"),</v>
+      </c>
+    </row>
+    <row r="3811" spans="1:5">
+      <c r="A3811">
+        <f t="shared" si="119"/>
+        <v>3810</v>
+      </c>
+      <c r="B3811" s="13">
+        <v>10</v>
+      </c>
+      <c r="C3811" t="s">
+        <v>3963</v>
+      </c>
+      <c r="D3811" s="6" t="s">
+        <v>3984</v>
+      </c>
+      <c r="E3811" t="str">
+        <f t="shared" si="120"/>
+        <v>("3810","10","lowest","أدنى"),</v>
+      </c>
+    </row>
+    <row r="3812" spans="1:5">
+      <c r="A3812">
+        <f t="shared" si="119"/>
+        <v>3811</v>
+      </c>
+      <c r="B3812" s="13">
+        <v>1</v>
+      </c>
+      <c r="C3812" t="s">
+        <v>3964</v>
+      </c>
+      <c r="D3812" s="6" t="s">
+        <v>3985</v>
+      </c>
+      <c r="E3812" t="str">
+        <f t="shared" si="120"/>
+        <v>("3811","1","daily","Daily"),</v>
+      </c>
+    </row>
+    <row r="3813" spans="1:5">
+      <c r="A3813">
+        <f t="shared" si="119"/>
+        <v>3812</v>
+      </c>
+      <c r="B3813" s="13">
+        <v>2</v>
+      </c>
+      <c r="C3813" t="s">
+        <v>3964</v>
+      </c>
+      <c r="D3813" s="6" t="s">
+        <v>3989</v>
+      </c>
+      <c r="E3813" t="str">
+        <f t="shared" si="120"/>
+        <v>("3812","2","daily","தினசரி"),</v>
+      </c>
+    </row>
+    <row r="3814" spans="1:5">
+      <c r="A3814">
+        <f t="shared" si="119"/>
+        <v>3813</v>
+      </c>
+      <c r="B3814" s="13">
+        <v>3</v>
+      </c>
+      <c r="C3814" t="s">
+        <v>3964</v>
+      </c>
+      <c r="D3814" s="6" t="s">
+        <v>3990</v>
+      </c>
+      <c r="E3814" t="str">
+        <f t="shared" si="120"/>
+        <v>("3813","3","daily","du quotidien"),</v>
+      </c>
+    </row>
+    <row r="3815" spans="1:5">
+      <c r="A3815">
+        <f t="shared" si="119"/>
+        <v>3814</v>
+      </c>
+      <c r="B3815" s="13">
+        <v>4</v>
+      </c>
+      <c r="C3815" t="s">
+        <v>3964</v>
+      </c>
+      <c r="D3815" s="6" t="s">
+        <v>3991</v>
+      </c>
+      <c r="E3815" t="str">
+        <f t="shared" si="120"/>
+        <v>("3814","4","daily","日常的"),</v>
+      </c>
+    </row>
+    <row r="3816" spans="1:5">
+      <c r="A3816">
+        <f t="shared" si="119"/>
+        <v>3815</v>
+      </c>
+      <c r="B3816" s="13">
+        <v>5</v>
+      </c>
+      <c r="C3816" t="s">
+        <v>3964</v>
+      </c>
+      <c r="D3816" s="6" t="s">
+        <v>3988</v>
+      </c>
+      <c r="E3816" t="str">
+        <f t="shared" si="120"/>
+        <v>("3815","5","daily","毎日"),</v>
+      </c>
+    </row>
+    <row r="3817" spans="1:5">
+      <c r="A3817">
+        <f t="shared" si="119"/>
+        <v>3816</v>
+      </c>
+      <c r="B3817" s="13">
+        <v>6</v>
+      </c>
+      <c r="C3817" t="s">
+        <v>3964</v>
+      </c>
+      <c r="D3817" s="6" t="s">
+        <v>3987</v>
+      </c>
+      <c r="E3817" t="str">
+        <f t="shared" si="120"/>
+        <v>("3816","6","daily","diário"),</v>
+      </c>
+    </row>
+    <row r="3818" spans="1:5">
+      <c r="A3818">
+        <f t="shared" si="119"/>
+        <v>3817</v>
+      </c>
+      <c r="B3818" s="13">
+        <v>7</v>
+      </c>
+      <c r="C3818" t="s">
+        <v>3964</v>
+      </c>
+      <c r="D3818" s="6" t="s">
+        <v>3992</v>
+      </c>
+      <c r="E3818" t="str">
+        <f t="shared" si="120"/>
+        <v>("3817","7","daily","रोज"),</v>
+      </c>
+    </row>
+    <row r="3819" spans="1:5">
+      <c r="A3819">
+        <f t="shared" si="119"/>
+        <v>3818</v>
+      </c>
+      <c r="B3819" s="13">
+        <v>8</v>
+      </c>
+      <c r="C3819" t="s">
+        <v>3964</v>
+      </c>
+      <c r="D3819" s="6" t="s">
+        <v>3993</v>
+      </c>
+      <c r="E3819" t="str">
+        <f t="shared" si="120"/>
+        <v>("3818","8","daily","повседневная"),</v>
+      </c>
+    </row>
+    <row r="3820" spans="1:5">
+      <c r="A3820">
+        <f t="shared" si="119"/>
+        <v>3819</v>
+      </c>
+      <c r="B3820" s="13">
+        <v>9</v>
+      </c>
+      <c r="C3820" t="s">
+        <v>3964</v>
+      </c>
+      <c r="D3820" s="6" t="s">
+        <v>3994</v>
+      </c>
+      <c r="E3820" t="str">
+        <f t="shared" si="120"/>
+        <v>("3819","9","daily","Diario"),</v>
+      </c>
+    </row>
+    <row r="3821" spans="1:5">
+      <c r="A3821">
+        <f t="shared" si="119"/>
+        <v>3820</v>
+      </c>
+      <c r="B3821" s="13">
+        <v>10</v>
+      </c>
+      <c r="C3821" t="s">
+        <v>3964</v>
+      </c>
+      <c r="D3821" t="s">
+        <v>3986</v>
+      </c>
+      <c r="E3821" t="str">
+        <f t="shared" si="120"/>
+        <v>("3820","10","daily","اليومي"),</v>
+      </c>
+    </row>
+    <row r="3822" spans="1:5">
+      <c r="A3822">
+        <f t="shared" si="119"/>
+        <v>3821</v>
+      </c>
+      <c r="B3822" s="13">
+        <v>1</v>
+      </c>
+      <c r="C3822" t="s">
+        <v>3965</v>
+      </c>
+      <c r="D3822" s="6" t="s">
+        <v>3995</v>
+      </c>
+      <c r="E3822" t="str">
+        <f t="shared" si="120"/>
+        <v>("3821","1","hourly","Hourly"),</v>
+      </c>
+    </row>
+    <row r="3823" spans="1:5">
+      <c r="A3823">
+        <f t="shared" si="119"/>
+        <v>3822</v>
+      </c>
+      <c r="B3823" s="13">
+        <v>2</v>
+      </c>
+      <c r="C3823" t="s">
+        <v>3965</v>
+      </c>
+      <c r="D3823" s="6" t="s">
+        <v>3999</v>
+      </c>
+      <c r="E3823" t="str">
+        <f t="shared" si="120"/>
+        <v>("3822","2","hourly","மணிக்கு "),</v>
+      </c>
+    </row>
+    <row r="3824" spans="1:5">
+      <c r="A3824">
+        <f t="shared" si="119"/>
+        <v>3823</v>
+      </c>
+      <c r="B3824" s="13">
+        <v>3</v>
+      </c>
+      <c r="C3824" t="s">
+        <v>3965</v>
+      </c>
+      <c r="D3824" s="6" t="s">
+        <v>4000</v>
+      </c>
+      <c r="E3824" t="str">
+        <f t="shared" si="120"/>
+        <v>("3823","3","hourly","toutes les heures"),</v>
+      </c>
+    </row>
+    <row r="3825" spans="1:5">
+      <c r="A3825">
+        <f t="shared" si="119"/>
+        <v>3824</v>
+      </c>
+      <c r="B3825" s="13">
+        <v>4</v>
+      </c>
+      <c r="C3825" t="s">
+        <v>3965</v>
+      </c>
+      <c r="D3825" s="6" t="s">
+        <v>4001</v>
+      </c>
+      <c r="E3825" t="str">
+        <f t="shared" si="120"/>
+        <v>("3824","4","hourly","每小时"),</v>
+      </c>
+    </row>
+    <row r="3826" spans="1:5">
+      <c r="A3826">
+        <f t="shared" si="119"/>
+        <v>3825</v>
+      </c>
+      <c r="B3826" s="13">
+        <v>5</v>
+      </c>
+      <c r="C3826" t="s">
+        <v>3965</v>
+      </c>
+      <c r="D3826" s="6" t="s">
+        <v>4002</v>
+      </c>
+      <c r="E3826" t="str">
+        <f t="shared" si="120"/>
+        <v>("3825","5","hourly","毎時"),</v>
+      </c>
+    </row>
+    <row r="3827" spans="1:5">
+      <c r="A3827">
+        <f t="shared" si="119"/>
+        <v>3826</v>
+      </c>
+      <c r="B3827" s="13">
+        <v>6</v>
+      </c>
+      <c r="C3827" t="s">
+        <v>3965</v>
+      </c>
+      <c r="D3827" s="6" t="s">
+        <v>4003</v>
+      </c>
+      <c r="E3827" t="str">
+        <f t="shared" si="120"/>
+        <v>("3826","6","hourly","de hora em hora"),</v>
+      </c>
+    </row>
+    <row r="3828" spans="1:5">
+      <c r="A3828">
+        <f t="shared" si="119"/>
+        <v>3827</v>
+      </c>
+      <c r="B3828" s="13">
+        <v>7</v>
+      </c>
+      <c r="C3828" t="s">
+        <v>3965</v>
+      </c>
+      <c r="D3828" s="6" t="s">
+        <v>3998</v>
+      </c>
+      <c r="E3828" t="str">
+        <f t="shared" si="120"/>
+        <v>("3827","7","hourly","प्रति घंटा"),</v>
+      </c>
+    </row>
+    <row r="3829" spans="1:5">
+      <c r="A3829">
+        <f t="shared" si="119"/>
+        <v>3828</v>
+      </c>
+      <c r="B3829" s="13">
+        <v>8</v>
+      </c>
+      <c r="C3829" t="s">
+        <v>3965</v>
+      </c>
+      <c r="D3829" s="6" t="s">
+        <v>3997</v>
+      </c>
+      <c r="E3829" t="str">
+        <f t="shared" si="120"/>
+        <v>("3828","8","hourly","ежечасно"),</v>
+      </c>
+    </row>
+    <row r="3830" spans="1:5">
+      <c r="A3830">
+        <f t="shared" si="119"/>
+        <v>3829</v>
+      </c>
+      <c r="B3830" s="13">
+        <v>9</v>
+      </c>
+      <c r="C3830" t="s">
+        <v>3965</v>
+      </c>
+      <c r="D3830" s="6" t="s">
+        <v>3996</v>
+      </c>
+      <c r="E3830" t="str">
+        <f t="shared" si="120"/>
+        <v>("3829","9","hourly","cada hora"),</v>
+      </c>
+    </row>
+    <row r="3831" spans="1:5">
+      <c r="A3831">
+        <f t="shared" si="119"/>
+        <v>3830</v>
+      </c>
+      <c r="B3831" s="13">
+        <v>10</v>
+      </c>
+      <c r="C3831" t="s">
+        <v>3965</v>
+      </c>
+      <c r="D3831" s="6" t="s">
+        <v>4004</v>
+      </c>
+      <c r="E3831" t="str">
+        <f t="shared" si="120"/>
+        <v>("3830","10","hourly","ساعيا"),</v>
+      </c>
+    </row>
+    <row r="3832" spans="1:5">
+      <c r="A3832">
+        <f t="shared" si="119"/>
+        <v>3831</v>
+      </c>
+      <c r="B3832" s="13">
+        <v>1</v>
+      </c>
+      <c r="C3832" t="s">
+        <v>3966</v>
+      </c>
+      <c r="D3832" s="6" t="s">
+        <v>4005</v>
+      </c>
+      <c r="E3832" t="str">
+        <f t="shared" si="120"/>
+        <v>("3831","1","weekly","Weekly"),</v>
+      </c>
+    </row>
+    <row r="3833" spans="1:5">
+      <c r="A3833">
+        <f t="shared" ref="A3833:A3841" si="121">A3832+1</f>
+        <v>3832</v>
+      </c>
+      <c r="B3833" s="13">
+        <v>2</v>
+      </c>
+      <c r="C3833" t="s">
+        <v>3966</v>
+      </c>
+      <c r="D3833" s="6" t="s">
+        <v>4009</v>
+      </c>
+      <c r="E3833" t="str">
+        <f t="shared" ref="E3833:E3841" si="122">CONCATENATE("(",CHAR(34),A3833,CHAR(34),",",CHAR(34),B3833,CHAR(34),",",CHAR(34),C3833,CHAR(34),",",CHAR(34),D3833,CHAR(34),"),")</f>
+        <v>("3832","2","weekly","வாரந்தோறும்"),</v>
+      </c>
+    </row>
+    <row r="3834" spans="1:5">
+      <c r="A3834">
+        <f t="shared" si="121"/>
+        <v>3833</v>
+      </c>
+      <c r="B3834" s="13">
+        <v>3</v>
+      </c>
+      <c r="C3834" t="s">
+        <v>3966</v>
+      </c>
+      <c r="D3834" s="6" t="s">
+        <v>4010</v>
+      </c>
+      <c r="E3834" t="str">
+        <f t="shared" si="122"/>
+        <v>("3833","3","weekly","hebdomadaire"),</v>
+      </c>
+    </row>
+    <row r="3835" spans="1:5">
+      <c r="A3835">
+        <f t="shared" si="121"/>
+        <v>3834</v>
+      </c>
+      <c r="B3835" s="13">
+        <v>4</v>
+      </c>
+      <c r="C3835" t="s">
+        <v>3966</v>
+      </c>
+      <c r="D3835" s="6" t="s">
+        <v>4011</v>
+      </c>
+      <c r="E3835" t="str">
+        <f t="shared" si="122"/>
+        <v>("3834","4","weekly","每周"),</v>
+      </c>
+    </row>
+    <row r="3836" spans="1:5">
+      <c r="A3836">
+        <f t="shared" si="121"/>
+        <v>3835</v>
+      </c>
+      <c r="B3836" s="13">
+        <v>5</v>
+      </c>
+      <c r="C3836" t="s">
+        <v>3966</v>
+      </c>
+      <c r="D3836" s="6" t="s">
+        <v>4008</v>
+      </c>
+      <c r="E3836" t="str">
+        <f t="shared" si="122"/>
+        <v>("3835","5","weekly","毎週"),</v>
+      </c>
+    </row>
+    <row r="3837" spans="1:5">
+      <c r="A3837">
+        <f t="shared" si="121"/>
+        <v>3836</v>
+      </c>
+      <c r="B3837" s="13">
+        <v>6</v>
+      </c>
+      <c r="C3837" t="s">
+        <v>3966</v>
+      </c>
+      <c r="D3837" s="6" t="s">
+        <v>4007</v>
+      </c>
+      <c r="E3837" t="str">
+        <f t="shared" si="122"/>
+        <v>("3836","6","weekly","semanalmente"),</v>
+      </c>
+    </row>
+    <row r="3838" spans="1:5">
+      <c r="A3838">
+        <f t="shared" si="121"/>
+        <v>3837</v>
+      </c>
+      <c r="B3838" s="13">
+        <v>7</v>
+      </c>
+      <c r="C3838" t="s">
+        <v>3966</v>
+      </c>
+      <c r="D3838" s="6" t="s">
+        <v>4012</v>
+      </c>
+      <c r="E3838" t="str">
+        <f t="shared" si="122"/>
+        <v>("3837","7","weekly","साप्ताहिक"),</v>
+      </c>
+    </row>
+    <row r="3839" spans="1:5">
+      <c r="A3839">
+        <f t="shared" si="121"/>
+        <v>3838</v>
+      </c>
+      <c r="B3839" s="13">
+        <v>8</v>
+      </c>
+      <c r="C3839" t="s">
+        <v>3966</v>
+      </c>
+      <c r="D3839" s="6" t="s">
+        <v>4013</v>
+      </c>
+      <c r="E3839" t="str">
+        <f t="shared" si="122"/>
+        <v>("3838","8","weekly","еженедельно"),</v>
+      </c>
+    </row>
+    <row r="3840" spans="1:5">
+      <c r="A3840">
+        <f t="shared" si="121"/>
+        <v>3839</v>
+      </c>
+      <c r="B3840" s="13">
+        <v>9</v>
+      </c>
+      <c r="C3840" t="s">
+        <v>3966</v>
+      </c>
+      <c r="D3840" s="6" t="s">
+        <v>4007</v>
+      </c>
+      <c r="E3840" t="str">
+        <f t="shared" si="122"/>
+        <v>("3839","9","weekly","semanalmente"),</v>
+      </c>
+    </row>
+    <row r="3841" spans="1:5">
+      <c r="A3841">
+        <f t="shared" si="121"/>
+        <v>3840</v>
+      </c>
+      <c r="B3841" s="13">
+        <v>10</v>
+      </c>
+      <c r="C3841" t="s">
+        <v>3966</v>
+      </c>
+      <c r="D3841" s="6" t="s">
+        <v>4006</v>
+      </c>
+      <c r="E3841" t="str">
+        <f t="shared" si="122"/>
+        <v>("3840","10","weekly","أسبوعي"),</v>
+      </c>
+    </row>
+    <row r="3842" spans="1:5">
+      <c r="E3842" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="3793" spans="5:5" ht="17">
-      <c r="E3793" s="5" t="s">
+    <row r="3843" spans="1:5" ht="17">
+      <c r="E3843" s="5" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="3794" spans="5:5" ht="17">
-      <c r="E3794" s="5" t="s">
+    <row r="3844" spans="1:5" ht="17">
+      <c r="E3844" s="5" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="3795" spans="5:5" ht="17">
-      <c r="E3795" s="5" t="s">
+    <row r="3845" spans="1:5" ht="17">
+      <c r="E3845" s="5" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="3796" spans="5:5">
-      <c r="E3796" s="6" t="s">
+    <row r="3846" spans="1:5">
+      <c r="E3846" s="6" t="s">
         <v>1033</v>
       </c>
     </row>
-    <row r="3797" spans="5:5" ht="17">
-      <c r="E3797" s="5" t="s">
+    <row r="3847" spans="1:5" ht="17">
+      <c r="E3847" s="5" t="s">
         <v>515</v>
       </c>
     </row>
-    <row r="3798" spans="5:5" ht="17">
-      <c r="E3798" s="5" t="s">
+    <row r="3848" spans="1:5" ht="17">
+      <c r="E3848" s="5" t="s">
         <v>516</v>
       </c>
     </row>
-    <row r="3799" spans="5:5" ht="17">
-      <c r="E3799" s="5" t="s">
+    <row r="3849" spans="1:5" ht="17">
+      <c r="E3849" s="5" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="3800" spans="5:5" ht="17">
-      <c r="E3800" s="5" t="s">
+    <row r="3850" spans="1:5" ht="17">
+      <c r="E3850" s="5" t="s">
         <v>1445</v>
       </c>
     </row>
-    <row r="3801" spans="5:5" ht="17">
-      <c r="E3801" s="5" t="s">
+    <row r="3851" spans="1:5" ht="17">
+      <c r="E3851" s="5" t="s">
         <v>3819</v>
       </c>
     </row>

</xml_diff>

<commit_message>
inc metric bug fix
</commit_message>
<xml_diff>
--- a/i18n.xlsx
+++ b/i18n.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/moneyPlanner/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{519E1FFF-5CB9-B643-AAC1-A320866AFFE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FEDCE96-88C9-E84F-B9E8-820D36EF5541}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1780" yWindow="500" windowWidth="33600" windowHeight="19040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="i18n" sheetId="1" r:id="rId1"/>
@@ -11963,9 +11963,6 @@
     <t>Highest</t>
   </si>
   <si>
-    <t>மிக உயர்ந்தது</t>
-  </si>
-  <si>
     <t>最高</t>
   </si>
   <si>
@@ -12099,6 +12096,9 @@
   </si>
   <si>
     <t>еженедельно</t>
+  </si>
+  <si>
+    <t>உயர்ந்த</t>
   </si>
 </sst>
 </file>
@@ -13052,8 +13052,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F3851"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3818" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E3846" sqref="E3846"/>
+    <sheetView tabSelected="1" topLeftCell="A1436" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C1452" sqref="C1452"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -85134,11 +85134,11 @@
         <v>3962</v>
       </c>
       <c r="D3793" s="6" t="s">
-        <v>3968</v>
+        <v>4013</v>
       </c>
       <c r="E3793" t="str">
         <f t="shared" si="120"/>
-        <v>("3792","2","highest","மிக உயர்ந்தது"),</v>
+        <v>("3792","2","highest","உயர்ந்த"),</v>
       </c>
     </row>
     <row r="3794" spans="1:5">
@@ -85153,7 +85153,7 @@
         <v>3962</v>
       </c>
       <c r="D3794" s="6" t="s">
-        <v>3971</v>
+        <v>3970</v>
       </c>
       <c r="E3794" t="str">
         <f t="shared" si="120"/>
@@ -85172,7 +85172,7 @@
         <v>3962</v>
       </c>
       <c r="D3795" s="6" t="s">
-        <v>3969</v>
+        <v>3968</v>
       </c>
       <c r="E3795" t="str">
         <f t="shared" si="120"/>
@@ -85191,7 +85191,7 @@
         <v>3962</v>
       </c>
       <c r="D3796" s="6" t="s">
-        <v>3969</v>
+        <v>3968</v>
       </c>
       <c r="E3796" t="str">
         <f t="shared" si="120"/>
@@ -85210,7 +85210,7 @@
         <v>3962</v>
       </c>
       <c r="D3797" s="6" t="s">
-        <v>3972</v>
+        <v>3971</v>
       </c>
       <c r="E3797" t="str">
         <f t="shared" si="120"/>
@@ -85229,7 +85229,7 @@
         <v>3962</v>
       </c>
       <c r="D3798" s="6" t="s">
-        <v>3973</v>
+        <v>3972</v>
       </c>
       <c r="E3798" t="str">
         <f t="shared" si="120"/>
@@ -85248,7 +85248,7 @@
         <v>3962</v>
       </c>
       <c r="D3799" s="6" t="s">
-        <v>3974</v>
+        <v>3973</v>
       </c>
       <c r="E3799" t="str">
         <f t="shared" si="120"/>
@@ -85267,7 +85267,7 @@
         <v>3962</v>
       </c>
       <c r="D3800" s="6" t="s">
-        <v>3975</v>
+        <v>3974</v>
       </c>
       <c r="E3800" t="str">
         <f t="shared" si="120"/>
@@ -85286,7 +85286,7 @@
         <v>3962</v>
       </c>
       <c r="D3801" s="6" t="s">
-        <v>3970</v>
+        <v>3969</v>
       </c>
       <c r="E3801" t="str">
         <f t="shared" si="120"/>
@@ -85305,7 +85305,7 @@
         <v>3963</v>
       </c>
       <c r="D3802" s="6" t="s">
-        <v>3976</v>
+        <v>3975</v>
       </c>
       <c r="E3802" t="str">
         <f t="shared" si="120"/>
@@ -85324,7 +85324,7 @@
         <v>3963</v>
       </c>
       <c r="D3803" s="6" t="s">
-        <v>3980</v>
+        <v>3979</v>
       </c>
       <c r="E3803" t="str">
         <f t="shared" si="120"/>
@@ -85343,7 +85343,7 @@
         <v>3963</v>
       </c>
       <c r="D3804" s="6" t="s">
-        <v>3981</v>
+        <v>3980</v>
       </c>
       <c r="E3804" t="str">
         <f t="shared" si="120"/>
@@ -85362,7 +85362,7 @@
         <v>3963</v>
       </c>
       <c r="D3805" s="6" t="s">
-        <v>3982</v>
+        <v>3981</v>
       </c>
       <c r="E3805" t="str">
         <f t="shared" si="120"/>
@@ -85381,7 +85381,7 @@
         <v>3963</v>
       </c>
       <c r="D3806" s="6" t="s">
-        <v>3982</v>
+        <v>3981</v>
       </c>
       <c r="E3806" t="str">
         <f t="shared" si="120"/>
@@ -85400,7 +85400,7 @@
         <v>3963</v>
       </c>
       <c r="D3807" s="6" t="s">
-        <v>3983</v>
+        <v>3982</v>
       </c>
       <c r="E3807" t="str">
         <f t="shared" si="120"/>
@@ -85419,7 +85419,7 @@
         <v>3963</v>
       </c>
       <c r="D3808" s="6" t="s">
-        <v>3979</v>
+        <v>3978</v>
       </c>
       <c r="E3808" t="str">
         <f t="shared" si="120"/>
@@ -85438,7 +85438,7 @@
         <v>3963</v>
       </c>
       <c r="D3809" s="6" t="s">
-        <v>3978</v>
+        <v>3977</v>
       </c>
       <c r="E3809" t="str">
         <f t="shared" si="120"/>
@@ -85457,7 +85457,7 @@
         <v>3963</v>
       </c>
       <c r="D3810" s="6" t="s">
-        <v>3977</v>
+        <v>3976</v>
       </c>
       <c r="E3810" t="str">
         <f t="shared" si="120"/>
@@ -85476,7 +85476,7 @@
         <v>3963</v>
       </c>
       <c r="D3811" s="6" t="s">
-        <v>3984</v>
+        <v>3983</v>
       </c>
       <c r="E3811" t="str">
         <f t="shared" si="120"/>
@@ -85495,7 +85495,7 @@
         <v>3964</v>
       </c>
       <c r="D3812" s="6" t="s">
-        <v>3985</v>
+        <v>3984</v>
       </c>
       <c r="E3812" t="str">
         <f t="shared" si="120"/>
@@ -85514,7 +85514,7 @@
         <v>3964</v>
       </c>
       <c r="D3813" s="6" t="s">
-        <v>3989</v>
+        <v>3988</v>
       </c>
       <c r="E3813" t="str">
         <f t="shared" si="120"/>
@@ -85533,7 +85533,7 @@
         <v>3964</v>
       </c>
       <c r="D3814" s="6" t="s">
-        <v>3990</v>
+        <v>3989</v>
       </c>
       <c r="E3814" t="str">
         <f t="shared" si="120"/>
@@ -85552,7 +85552,7 @@
         <v>3964</v>
       </c>
       <c r="D3815" s="6" t="s">
-        <v>3991</v>
+        <v>3990</v>
       </c>
       <c r="E3815" t="str">
         <f t="shared" si="120"/>
@@ -85571,7 +85571,7 @@
         <v>3964</v>
       </c>
       <c r="D3816" s="6" t="s">
-        <v>3988</v>
+        <v>3987</v>
       </c>
       <c r="E3816" t="str">
         <f t="shared" si="120"/>
@@ -85590,7 +85590,7 @@
         <v>3964</v>
       </c>
       <c r="D3817" s="6" t="s">
-        <v>3987</v>
+        <v>3986</v>
       </c>
       <c r="E3817" t="str">
         <f t="shared" si="120"/>
@@ -85609,7 +85609,7 @@
         <v>3964</v>
       </c>
       <c r="D3818" s="6" t="s">
-        <v>3992</v>
+        <v>3991</v>
       </c>
       <c r="E3818" t="str">
         <f t="shared" si="120"/>
@@ -85628,7 +85628,7 @@
         <v>3964</v>
       </c>
       <c r="D3819" s="6" t="s">
-        <v>3993</v>
+        <v>3992</v>
       </c>
       <c r="E3819" t="str">
         <f t="shared" si="120"/>
@@ -85647,7 +85647,7 @@
         <v>3964</v>
       </c>
       <c r="D3820" s="6" t="s">
-        <v>3994</v>
+        <v>3993</v>
       </c>
       <c r="E3820" t="str">
         <f t="shared" si="120"/>
@@ -85666,7 +85666,7 @@
         <v>3964</v>
       </c>
       <c r="D3821" t="s">
-        <v>3986</v>
+        <v>3985</v>
       </c>
       <c r="E3821" t="str">
         <f t="shared" si="120"/>
@@ -85685,7 +85685,7 @@
         <v>3965</v>
       </c>
       <c r="D3822" s="6" t="s">
-        <v>3995</v>
+        <v>3994</v>
       </c>
       <c r="E3822" t="str">
         <f t="shared" si="120"/>
@@ -85704,7 +85704,7 @@
         <v>3965</v>
       </c>
       <c r="D3823" s="6" t="s">
-        <v>3999</v>
+        <v>3998</v>
       </c>
       <c r="E3823" t="str">
         <f t="shared" si="120"/>
@@ -85723,7 +85723,7 @@
         <v>3965</v>
       </c>
       <c r="D3824" s="6" t="s">
-        <v>4000</v>
+        <v>3999</v>
       </c>
       <c r="E3824" t="str">
         <f t="shared" si="120"/>
@@ -85742,7 +85742,7 @@
         <v>3965</v>
       </c>
       <c r="D3825" s="6" t="s">
-        <v>4001</v>
+        <v>4000</v>
       </c>
       <c r="E3825" t="str">
         <f t="shared" si="120"/>
@@ -85761,7 +85761,7 @@
         <v>3965</v>
       </c>
       <c r="D3826" s="6" t="s">
-        <v>4002</v>
+        <v>4001</v>
       </c>
       <c r="E3826" t="str">
         <f t="shared" si="120"/>
@@ -85780,7 +85780,7 @@
         <v>3965</v>
       </c>
       <c r="D3827" s="6" t="s">
-        <v>4003</v>
+        <v>4002</v>
       </c>
       <c r="E3827" t="str">
         <f t="shared" si="120"/>
@@ -85799,7 +85799,7 @@
         <v>3965</v>
       </c>
       <c r="D3828" s="6" t="s">
-        <v>3998</v>
+        <v>3997</v>
       </c>
       <c r="E3828" t="str">
         <f t="shared" si="120"/>
@@ -85818,7 +85818,7 @@
         <v>3965</v>
       </c>
       <c r="D3829" s="6" t="s">
-        <v>3997</v>
+        <v>3996</v>
       </c>
       <c r="E3829" t="str">
         <f t="shared" si="120"/>
@@ -85837,7 +85837,7 @@
         <v>3965</v>
       </c>
       <c r="D3830" s="6" t="s">
-        <v>3996</v>
+        <v>3995</v>
       </c>
       <c r="E3830" t="str">
         <f t="shared" si="120"/>
@@ -85856,7 +85856,7 @@
         <v>3965</v>
       </c>
       <c r="D3831" s="6" t="s">
-        <v>4004</v>
+        <v>4003</v>
       </c>
       <c r="E3831" t="str">
         <f t="shared" si="120"/>
@@ -85875,7 +85875,7 @@
         <v>3966</v>
       </c>
       <c r="D3832" s="6" t="s">
-        <v>4005</v>
+        <v>4004</v>
       </c>
       <c r="E3832" t="str">
         <f t="shared" si="120"/>
@@ -85894,7 +85894,7 @@
         <v>3966</v>
       </c>
       <c r="D3833" s="6" t="s">
-        <v>4009</v>
+        <v>4008</v>
       </c>
       <c r="E3833" t="str">
         <f t="shared" ref="E3833:E3841" si="122">CONCATENATE("(",CHAR(34),A3833,CHAR(34),",",CHAR(34),B3833,CHAR(34),",",CHAR(34),C3833,CHAR(34),",",CHAR(34),D3833,CHAR(34),"),")</f>
@@ -85913,7 +85913,7 @@
         <v>3966</v>
       </c>
       <c r="D3834" s="6" t="s">
-        <v>4010</v>
+        <v>4009</v>
       </c>
       <c r="E3834" t="str">
         <f t="shared" si="122"/>
@@ -85932,7 +85932,7 @@
         <v>3966</v>
       </c>
       <c r="D3835" s="6" t="s">
-        <v>4011</v>
+        <v>4010</v>
       </c>
       <c r="E3835" t="str">
         <f t="shared" si="122"/>
@@ -85951,7 +85951,7 @@
         <v>3966</v>
       </c>
       <c r="D3836" s="6" t="s">
-        <v>4008</v>
+        <v>4007</v>
       </c>
       <c r="E3836" t="str">
         <f t="shared" si="122"/>
@@ -85970,7 +85970,7 @@
         <v>3966</v>
       </c>
       <c r="D3837" s="6" t="s">
-        <v>4007</v>
+        <v>4006</v>
       </c>
       <c r="E3837" t="str">
         <f t="shared" si="122"/>
@@ -85989,7 +85989,7 @@
         <v>3966</v>
       </c>
       <c r="D3838" s="6" t="s">
-        <v>4012</v>
+        <v>4011</v>
       </c>
       <c r="E3838" t="str">
         <f t="shared" si="122"/>
@@ -86008,7 +86008,7 @@
         <v>3966</v>
       </c>
       <c r="D3839" s="6" t="s">
-        <v>4013</v>
+        <v>4012</v>
       </c>
       <c r="E3839" t="str">
         <f t="shared" si="122"/>
@@ -86027,7 +86027,7 @@
         <v>3966</v>
       </c>
       <c r="D3840" s="6" t="s">
-        <v>4007</v>
+        <v>4006</v>
       </c>
       <c r="E3840" t="str">
         <f t="shared" si="122"/>
@@ -86046,7 +86046,7 @@
         <v>3966</v>
       </c>
       <c r="D3841" s="6" t="s">
-        <v>4006</v>
+        <v>4005</v>
       </c>
       <c r="E3841" t="str">
         <f t="shared" si="122"/>

</xml_diff>